<commit_message>
microarray and RNA-seq script edits
</commit_message>
<xml_diff>
--- a/DGEA/Pheno_microarrays.xlsx
+++ b/DGEA/Pheno_microarrays.xlsx
@@ -26,7 +26,7 @@
     <t xml:space="preserve">GSM4274195</t>
   </si>
   <si>
-    <t xml:space="preserve">non_tumor</t>
+    <t xml:space="preserve">normal</t>
   </si>
   <si>
     <t xml:space="preserve">GSE143754</t>
@@ -1656,7 +1656,9 @@
       <c r="A72" t="s">
         <v>80</v>
       </c>
-      <c r="B72"/>
+      <c r="B72" t="s">
+        <v>17</v>
+      </c>
       <c r="C72" t="s">
         <v>70</v>
       </c>
@@ -1665,7 +1667,9 @@
       <c r="A73" t="s">
         <v>81</v>
       </c>
-      <c r="B73"/>
+      <c r="B73" t="s">
+        <v>17</v>
+      </c>
       <c r="C73" t="s">
         <v>70</v>
       </c>
@@ -1674,7 +1678,9 @@
       <c r="A74" t="s">
         <v>82</v>
       </c>
-      <c r="B74"/>
+      <c r="B74" t="s">
+        <v>17</v>
+      </c>
       <c r="C74" t="s">
         <v>70</v>
       </c>
@@ -1683,7 +1689,9 @@
       <c r="A75" t="s">
         <v>83</v>
       </c>
-      <c r="B75"/>
+      <c r="B75" t="s">
+        <v>17</v>
+      </c>
       <c r="C75" t="s">
         <v>70</v>
       </c>
@@ -1692,7 +1700,9 @@
       <c r="A76" t="s">
         <v>84</v>
       </c>
-      <c r="B76"/>
+      <c r="B76" t="s">
+        <v>17</v>
+      </c>
       <c r="C76" t="s">
         <v>70</v>
       </c>
@@ -1701,7 +1711,9 @@
       <c r="A77" t="s">
         <v>85</v>
       </c>
-      <c r="B77"/>
+      <c r="B77" t="s">
+        <v>17</v>
+      </c>
       <c r="C77" t="s">
         <v>70</v>
       </c>
@@ -1710,7 +1722,9 @@
       <c r="A78" t="s">
         <v>86</v>
       </c>
-      <c r="B78"/>
+      <c r="B78" t="s">
+        <v>17</v>
+      </c>
       <c r="C78" t="s">
         <v>70</v>
       </c>
@@ -1719,7 +1733,9 @@
       <c r="A79" t="s">
         <v>87</v>
       </c>
-      <c r="B79"/>
+      <c r="B79" t="s">
+        <v>17</v>
+      </c>
       <c r="C79" t="s">
         <v>70</v>
       </c>
@@ -1728,7 +1744,9 @@
       <c r="A80" t="s">
         <v>88</v>
       </c>
-      <c r="B80"/>
+      <c r="B80" t="s">
+        <v>17</v>
+      </c>
       <c r="C80" t="s">
         <v>70</v>
       </c>
@@ -1737,7 +1755,9 @@
       <c r="A81" t="s">
         <v>89</v>
       </c>
-      <c r="B81"/>
+      <c r="B81" t="s">
+        <v>17</v>
+      </c>
       <c r="C81" t="s">
         <v>70</v>
       </c>

</xml_diff>